<commit_message>
Add scripts and run PPM+LSTM+PAQ8L
However, the DNA corpus is too large, so it is stored locally.
</commit_message>
<xml_diff>
--- a/Arithmetic/Results.xlsx
+++ b/Arithmetic/Results.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Documents\GitHub\DNA_Comp\Arithmetic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC6267AD-B552-45D4-ABC7-D12E37904369}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1386BD4-C8A7-407E-8AF5-75B2B1AEAF9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10248" yWindow="36" windowWidth="12732" windowHeight="12252" tabRatio="602" xr2:uid="{C9D022DD-FB2B-4FEA-BFA1-145DD998C539}"/>
+    <workbookView xWindow="12660" yWindow="0" windowWidth="13488" windowHeight="12252" tabRatio="602" xr2:uid="{C9D022DD-FB2B-4FEA-BFA1-145DD998C539}"/>
   </bookViews>
   <sheets>
     <sheet name="Result Table" sheetId="1" r:id="rId1"/>
-    <sheet name="Training Progress" sheetId="2" r:id="rId2"/>
+    <sheet name="Training Accuracy" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -24,7 +24,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="137">
   <si>
     <t>Model</t>
   </si>
@@ -440,6 +442,9 @@
   </si>
   <si>
     <t>NVIDIA Tesla K40c</t>
+  </si>
+  <si>
+    <t>CNNLSTM</t>
   </si>
 </sst>
 </file>
@@ -447,7 +452,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -481,7 +486,7 @@
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -492,7 +497,7 @@
   </cellStyles>
   <dxfs count="1">
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.000"/>
+      <numFmt numFmtId="164" formatCode="0.000"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -542,7 +547,16 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Performance Comparison during Training Ecoli</a:t>
+              <a:t>Performance Comparison</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t> during Online Training for Ecoli</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -587,7 +601,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Training Progress'!$C$23</c:f>
+              <c:f>'Training Accuracy'!$C$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -622,7 +636,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Training Progress'!$B$24:$B$33</c:f>
+              <c:f>'Training Accuracy'!$B$24:$B$33</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="10"/>
@@ -661,7 +675,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Training Progress'!$C$24:$C$33</c:f>
+              <c:f>'Training Accuracy'!$C$24:$C$33</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
@@ -710,7 +724,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Training Progress'!$D$23</c:f>
+              <c:f>'Training Accuracy'!$D$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -745,7 +759,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Training Progress'!$B$24:$B$33</c:f>
+              <c:f>'Training Accuracy'!$B$24:$B$33</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="10"/>
@@ -784,7 +798,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Training Progress'!$D$24:$D$33</c:f>
+              <c:f>'Training Accuracy'!$D$24:$D$33</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
@@ -833,7 +847,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Training Progress'!$E$23</c:f>
+              <c:f>'Training Accuracy'!$E$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -868,7 +882,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Training Progress'!$B$24:$B$33</c:f>
+              <c:f>'Training Accuracy'!$B$24:$B$33</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="10"/>
@@ -907,7 +921,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Training Progress'!$E$24:$E$33</c:f>
+              <c:f>'Training Accuracy'!$E$24:$E$33</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
@@ -956,7 +970,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Training Progress'!$F$23</c:f>
+              <c:f>'Training Accuracy'!$F$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -991,7 +1005,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Training Progress'!$B$24:$B$33</c:f>
+              <c:f>'Training Accuracy'!$B$24:$B$33</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1030,7 +1044,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Training Progress'!$F$24:$F$33</c:f>
+              <c:f>'Training Accuracy'!$F$24:$F$33</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1079,7 +1093,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Training Progress'!$G$23</c:f>
+              <c:f>'Training Accuracy'!$G$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1114,7 +1128,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Training Progress'!$B$24:$B$33</c:f>
+              <c:f>'Training Accuracy'!$B$24:$B$33</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1153,7 +1167,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Training Progress'!$G$24:$G$33</c:f>
+              <c:f>'Training Accuracy'!$G$24:$G$33</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1202,7 +1216,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Training Progress'!$H$23</c:f>
+              <c:f>'Training Accuracy'!$H$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1237,7 +1251,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Training Progress'!$B$24:$B$33</c:f>
+              <c:f>'Training Accuracy'!$B$24:$B$33</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1276,7 +1290,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Training Progress'!$H$24:$H$33</c:f>
+              <c:f>'Training Accuracy'!$H$24:$H$33</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1325,7 +1339,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Training Progress'!$I$23</c:f>
+              <c:f>'Training Accuracy'!$I$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1366,7 +1380,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Training Progress'!$B$24:$B$33</c:f>
+              <c:f>'Training Accuracy'!$B$24:$B$33</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1405,7 +1419,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Training Progress'!$I$24:$I$33</c:f>
+              <c:f>'Training Accuracy'!$I$24:$I$33</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
@@ -2300,8 +2314,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5F2351BE-3A98-4E7A-B54D-7F569A62826B}" name="Table1" displayName="Table1" ref="A5:M81" totalsRowShown="0">
-  <autoFilter ref="A5:M81" xr:uid="{96AABEC0-7C37-495E-B464-7FC807E4A945}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5F2351BE-3A98-4E7A-B54D-7F569A62826B}" name="Table1" displayName="Table1" ref="A5:M83" totalsRowShown="0">
+  <autoFilter ref="A5:M83" xr:uid="{96AABEC0-7C37-495E-B464-7FC807E4A945}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{D41ACE8B-D4C8-42D1-9C66-A864085CC195}" name="Model Family"/>
     <tableColumn id="2" xr3:uid="{1E3A58ED-E91C-4078-86E6-1AE504041D85}" name="Model"/>
@@ -2621,10 +2635,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2878EB5-10DC-401B-AF43-168E44053072}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A5:M81"/>
+  <dimension ref="A5:M83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M77" sqref="M77"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2705,7 +2719,7 @@
         <v>4638695</v>
       </c>
       <c r="I6" s="2">
-        <f>8*G6/E6</f>
+        <f t="shared" ref="I6:I37" si="0">8*G6/E6</f>
         <v>8</v>
       </c>
       <c r="J6" t="s">
@@ -2738,7 +2752,7 @@
         <v>1299059</v>
       </c>
       <c r="I7" s="2">
-        <f>8*G7/E7</f>
+        <f t="shared" si="0"/>
         <v>2.2403870053969919</v>
       </c>
       <c r="L7" t="s">
@@ -2762,7 +2776,7 @@
         <v>1251004</v>
       </c>
       <c r="I8" s="2">
-        <f>8*G8/E8</f>
+        <f t="shared" si="0"/>
         <v>2.1575102480331214</v>
       </c>
       <c r="L8" t="s">
@@ -2786,7 +2800,7 @@
         <v>1238459</v>
       </c>
       <c r="I9" s="2">
-        <f>8*G9/E9</f>
+        <f t="shared" si="0"/>
         <v>2.1358748527333655</v>
       </c>
       <c r="L9" t="s">
@@ -2813,7 +2827,7 @@
         <v>1102585</v>
       </c>
       <c r="I10" s="2">
-        <f>8*G10/E10</f>
+        <f t="shared" si="0"/>
         <v>1.9015434297792806</v>
       </c>
       <c r="L10" t="s">
@@ -2837,7 +2851,7 @@
         <v>1101724</v>
       </c>
       <c r="I11" s="2">
-        <f>8*G11/E11</f>
+        <f t="shared" si="0"/>
         <v>1.9000585293924261</v>
       </c>
       <c r="L11" t="s">
@@ -2861,7 +2875,7 @@
         <v>1115068</v>
       </c>
       <c r="I12" s="2">
-        <f>8*G12/E12</f>
+        <f t="shared" si="0"/>
         <v>1.9230718984541988</v>
       </c>
       <c r="L12" t="s">
@@ -2885,7 +2899,7 @@
         <v>1109862</v>
       </c>
       <c r="I13" s="2">
-        <f>8*G13/E13</f>
+        <f t="shared" si="0"/>
         <v>1.914093511213822</v>
       </c>
       <c r="L13" t="s">
@@ -2909,7 +2923,7 @@
         <v>1637985</v>
       </c>
       <c r="I14" s="2">
-        <f>8*G14/E14</f>
+        <f t="shared" si="0"/>
         <v>2.8249065739394377</v>
       </c>
       <c r="L14" t="s">
@@ -2933,8 +2947,11 @@
         <v>1114292</v>
       </c>
       <c r="I15" s="2">
-        <f>8*G15/E15</f>
+        <f t="shared" si="0"/>
         <v>1.9217335910207505</v>
+      </c>
+      <c r="J15">
+        <v>13</v>
       </c>
       <c r="L15" t="s">
         <v>134</v>
@@ -2954,7 +2971,7 @@
         <v>1165644</v>
       </c>
       <c r="I16" s="2">
-        <f>8*G16/E16</f>
+        <f t="shared" si="0"/>
         <v>2.0102964303537956</v>
       </c>
       <c r="L16" t="s">
@@ -2972,7 +2989,7 @@
         <v>1162480</v>
       </c>
       <c r="I17" s="2">
-        <f>8*G17/E17</f>
+        <f t="shared" si="0"/>
         <v>2.004839723241127</v>
       </c>
       <c r="L17" t="s">
@@ -2996,7 +3013,7 @@
         <v>1138627</v>
       </c>
       <c r="I18" s="2">
-        <f>8*G18/E18</f>
+        <f t="shared" si="0"/>
         <v>1.9637022912694195</v>
       </c>
       <c r="L18" t="s">
@@ -3023,7 +3040,7 @@
         <v>4638690</v>
       </c>
       <c r="I19" s="2">
-        <f>8*G19/E19</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="L19" t="s">
@@ -3047,7 +3064,7 @@
         <v>1325921</v>
       </c>
       <c r="I20" s="2">
-        <f>8*G20/E20</f>
+        <f t="shared" si="0"/>
         <v>2.2867162927464433</v>
       </c>
       <c r="L20" t="s">
@@ -3071,7 +3088,7 @@
         <v>1268262</v>
       </c>
       <c r="I21" s="2">
-        <f>8*G21/E21</f>
+        <f t="shared" si="0"/>
         <v>2.1872761490851942</v>
       </c>
       <c r="L21" t="s">
@@ -3095,7 +3112,7 @@
         <v>1267529</v>
       </c>
       <c r="I22" s="2">
-        <f>8*G22/E22</f>
+        <f t="shared" si="0"/>
         <v>2.1860119990773259</v>
       </c>
       <c r="L22" t="s">
@@ -3119,7 +3136,7 @@
         <v>1161904</v>
       </c>
       <c r="I23" s="2">
-        <f>8*G23/E23</f>
+        <f t="shared" si="0"/>
         <v>2.0038485003309123</v>
       </c>
       <c r="L23" t="s">
@@ -3140,7 +3157,7 @@
         <v>1167729</v>
       </c>
       <c r="I24" s="2">
-        <f>8*G24/E24</f>
+        <f t="shared" si="0"/>
         <v>2.0138944400250933</v>
       </c>
       <c r="L24" t="s">
@@ -3161,7 +3178,7 @@
         <v>1690549</v>
       </c>
       <c r="I25" s="2">
-        <f>8*G25/E25</f>
+        <f t="shared" si="0"/>
         <v>2.9155627989798845</v>
       </c>
       <c r="L25" t="s">
@@ -3182,7 +3199,7 @@
         <v>1163192</v>
       </c>
       <c r="I26" s="2">
-        <f>8*G26/E26</f>
+        <f t="shared" si="0"/>
         <v>2.0060698171250935</v>
       </c>
       <c r="L26" t="s">
@@ -3206,7 +3223,7 @@
         <v>1431685</v>
       </c>
       <c r="I27" s="2">
-        <f>8*G27/E27</f>
+        <f t="shared" si="0"/>
         <v>2.4691195143456448</v>
       </c>
       <c r="L27" t="s">
@@ -3227,7 +3244,7 @@
         <v>1165761</v>
       </c>
       <c r="I28" s="2">
-        <f>8*G28/E28</f>
+        <f t="shared" si="0"/>
         <v>2.0105003783395743</v>
       </c>
       <c r="L28" t="s">
@@ -3248,7 +3265,7 @@
         <v>1165702</v>
       </c>
       <c r="I29" s="2">
-        <f>8*G29/E29</f>
+        <f t="shared" si="0"/>
         <v>2.0103986254740023</v>
       </c>
       <c r="L29" t="s">
@@ -3266,7 +3283,7 @@
         <v>1162577</v>
       </c>
       <c r="I30" s="2">
-        <f>8*G30/E30</f>
+        <f t="shared" si="0"/>
         <v>2.0050091728483688</v>
       </c>
       <c r="L30" t="s">
@@ -3290,7 +3307,7 @@
         <v>1159829</v>
       </c>
       <c r="I31" s="2">
-        <f>8*G31/E31</f>
+        <f t="shared" si="0"/>
         <v>2.0002699037874918</v>
       </c>
       <c r="L31" t="s">
@@ -3309,7 +3326,7 @@
         <v>1161220</v>
       </c>
       <c r="I32" s="2">
-        <f>8*G32/E32</f>
+        <f t="shared" si="0"/>
         <v>2.0026688569402138</v>
       </c>
       <c r="L32" t="s">
@@ -3333,7 +3350,7 @@
         <v>1424590</v>
       </c>
       <c r="I33" s="2">
-        <f>8*G33/E33</f>
+        <f t="shared" si="0"/>
         <v>2.4568806528560296</v>
       </c>
       <c r="L33" t="s">
@@ -3354,7 +3371,7 @@
         <v>1165778</v>
       </c>
       <c r="I34" s="2">
-        <f>8*G34/E34</f>
+        <f t="shared" si="0"/>
         <v>2.0105275298332828</v>
       </c>
       <c r="L34" t="s">
@@ -3375,7 +3392,7 @@
         <v>1169095</v>
       </c>
       <c r="I35" s="2">
-        <f>8*G35/E35</f>
+        <f t="shared" si="0"/>
         <v>2.0162481042620821</v>
       </c>
       <c r="L35" t="s">
@@ -3420,7 +3437,7 @@
         <v>1151124</v>
       </c>
       <c r="I37" s="2">
-        <f>8*G37/E37</f>
+        <f t="shared" si="0"/>
         <v>1.9852549046660752</v>
       </c>
       <c r="L37" t="s">
@@ -3444,7 +3461,7 @@
         <v>1217974</v>
       </c>
       <c r="I38" s="2">
-        <f>8*G38/E38</f>
+        <f t="shared" ref="I38:I71" si="1">8*G38/E38</f>
         <v>2.1005459509625015</v>
       </c>
       <c r="L38" t="s">
@@ -3468,7 +3485,7 @@
         <v>1327415</v>
       </c>
       <c r="I39" s="2">
-        <f>8*G39/E39</f>
+        <f t="shared" si="1"/>
         <v>2.2892904146532591</v>
       </c>
       <c r="L39" t="s">
@@ -3492,7 +3509,7 @@
         <v>1150929</v>
       </c>
       <c r="I40" s="2">
-        <f>8*G40/E40</f>
+        <f t="shared" si="1"/>
         <v>1.9849186031847319</v>
       </c>
       <c r="L40" t="s">
@@ -3513,7 +3530,7 @@
         <v>1152230</v>
       </c>
       <c r="I41" s="2">
-        <f>8*G41/E41</f>
+        <f t="shared" si="1"/>
         <v>1.9871623376833356</v>
       </c>
       <c r="L41" t="s">
@@ -3537,7 +3554,7 @@
         <v>1211435</v>
       </c>
       <c r="I42" s="2">
-        <f>8*G42/E42</f>
+        <f t="shared" si="1"/>
         <v>2.089268641288121</v>
       </c>
       <c r="L42" t="s">
@@ -3561,7 +3578,7 @@
         <v>1221173</v>
       </c>
       <c r="I43" s="2">
-        <f>8*G43/E43</f>
+        <f t="shared" si="1"/>
         <v>2.1060630198795134</v>
       </c>
       <c r="L43" t="s">
@@ -3585,7 +3602,7 @@
         <v>1176852</v>
       </c>
       <c r="I44" s="2">
-        <f>8*G44/E44</f>
+        <f t="shared" si="1"/>
         <v>2.0296260047276227</v>
       </c>
       <c r="L44" t="s">
@@ -3609,7 +3626,7 @@
         <v>1147840</v>
       </c>
       <c r="I45" s="2">
-        <f>8*G45/E45</f>
+        <f t="shared" si="1"/>
         <v>1.979591242795657</v>
       </c>
       <c r="L45" t="s">
@@ -3633,7 +3650,7 @@
         <v>1138251</v>
       </c>
       <c r="I46" s="2">
-        <f>8*G46/E46</f>
+        <f t="shared" si="1"/>
         <v>1.9630538330284704</v>
       </c>
       <c r="L46" t="s">
@@ -3657,7 +3674,7 @@
         <v>1179672</v>
       </c>
       <c r="I47" s="2">
-        <f>8*G47/E47</f>
+        <f t="shared" si="1"/>
         <v>2.0344894415347419</v>
       </c>
       <c r="L47" t="s">
@@ -3681,7 +3698,7 @@
         <v>1173204</v>
       </c>
       <c r="I48" s="2">
-        <f>8*G48/E48</f>
+        <f t="shared" si="1"/>
         <v>2.0233345800920302</v>
       </c>
       <c r="L48" t="s">
@@ -3705,7 +3722,7 @@
         <v>1133963</v>
       </c>
       <c r="I49" s="2">
-        <f>8*G49/E49</f>
+        <f t="shared" si="1"/>
         <v>1.9556586496848791</v>
       </c>
       <c r="L49" t="s">
@@ -3713,30 +3730,25 @@
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>60</v>
-      </c>
       <c r="B50" t="s">
-        <v>61</v>
-      </c>
-      <c r="D50" t="s">
-        <v>45</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="C50" s="3"/>
       <c r="E50">
         <v>4638695</v>
       </c>
       <c r="G50">
-        <v>1130656</v>
+        <v>1120802</v>
       </c>
       <c r="I50" s="2">
         <f>8*G50/E50</f>
-        <v>1.949955321485892</v>
-      </c>
-      <c r="L50" t="s">
-        <v>134</v>
+        <v>1.9329608866286747</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>60</v>
+      </c>
       <c r="B51" t="s">
         <v>61</v>
       </c>
@@ -3747,47 +3759,41 @@
         <v>4638695</v>
       </c>
       <c r="G51">
+        <v>1130656</v>
+      </c>
+      <c r="I51" s="2">
+        <f t="shared" si="1"/>
+        <v>1.949955321485892</v>
+      </c>
+      <c r="L51" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B52" t="s">
+        <v>61</v>
+      </c>
+      <c r="D52" t="s">
+        <v>45</v>
+      </c>
+      <c r="E52">
+        <v>4638695</v>
+      </c>
+      <c r="G52">
         <v>1128797</v>
       </c>
-      <c r="I51" s="2">
-        <f>8*G51/E51</f>
+      <c r="I52" s="2">
+        <f t="shared" si="1"/>
         <v>1.946749247363752</v>
       </c>
-      <c r="L51" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
+      <c r="L52" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
         <v>63</v>
       </c>
-      <c r="B52" t="s">
-        <v>62</v>
-      </c>
-      <c r="D52" t="s">
-        <v>47</v>
-      </c>
-      <c r="E52">
-        <v>4638695</v>
-      </c>
-      <c r="G52">
-        <v>1118429</v>
-      </c>
-      <c r="I52" s="2">
-        <f>8*G52/E52</f>
-        <v>1.9288683562941733</v>
-      </c>
-      <c r="J52">
-        <v>163.41999999999999</v>
-      </c>
-      <c r="L52" t="s">
-        <v>134</v>
-      </c>
-      <c r="M52" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>62</v>
       </c>
@@ -3798,20 +3804,20 @@
         <v>4638695</v>
       </c>
       <c r="G53">
-        <v>1140565</v>
+        <v>1118429</v>
       </c>
       <c r="I53" s="2">
-        <f>8*G53/E53</f>
-        <v>1.967044610607078</v>
+        <f t="shared" si="1"/>
+        <v>1.9288683562941733</v>
       </c>
       <c r="J53">
-        <v>120.03</v>
+        <v>163.41999999999999</v>
       </c>
       <c r="L53" t="s">
         <v>134</v>
       </c>
       <c r="M53" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.3">
@@ -3825,20 +3831,20 @@
         <v>4638695</v>
       </c>
       <c r="G54">
-        <v>1111045</v>
+        <v>1140565</v>
       </c>
       <c r="I54" s="2">
-        <f>8*G54/E54</f>
-        <v>1.9161337402006384</v>
+        <f t="shared" si="1"/>
+        <v>1.967044610607078</v>
       </c>
       <c r="J54">
-        <v>72.540000000000006</v>
+        <v>120.03</v>
       </c>
       <c r="L54" t="s">
         <v>134</v>
       </c>
       <c r="M54" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.3">
@@ -3852,20 +3858,20 @@
         <v>4638695</v>
       </c>
       <c r="G55">
-        <v>1194606</v>
+        <v>1111045</v>
       </c>
       <c r="I55" s="2">
-        <f>8*G55/E55</f>
-        <v>2.0602449611366991</v>
+        <f t="shared" si="1"/>
+        <v>1.9161337402006384</v>
       </c>
       <c r="J55">
-        <v>7.01</v>
+        <v>72.540000000000006</v>
       </c>
       <c r="L55" t="s">
         <v>134</v>
       </c>
       <c r="M55" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.3">
@@ -3879,20 +3885,20 @@
         <v>4638695</v>
       </c>
       <c r="G56">
-        <v>1203370</v>
+        <v>1194606</v>
       </c>
       <c r="I56" s="2">
-        <f>8*G56/E56</f>
-        <v>2.0753595569443561</v>
+        <f t="shared" si="1"/>
+        <v>2.0602449611366991</v>
       </c>
       <c r="J56">
-        <v>2.7</v>
+        <v>7.01</v>
       </c>
       <c r="L56" t="s">
         <v>134</v>
       </c>
       <c r="M56" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.3">
@@ -3906,20 +3912,20 @@
         <v>4638695</v>
       </c>
       <c r="G57">
-        <v>1098677</v>
+        <v>1203370</v>
       </c>
       <c r="I57" s="2">
-        <f>8*G57/E57</f>
-        <v>1.8948036031685636</v>
+        <f t="shared" si="1"/>
+        <v>2.0753595569443561</v>
       </c>
       <c r="J57">
-        <v>2.27</v>
+        <v>2.7</v>
       </c>
       <c r="L57" t="s">
         <v>134</v>
       </c>
       <c r="M57" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.3">
@@ -3933,17 +3939,20 @@
         <v>4638695</v>
       </c>
       <c r="G58">
-        <v>1108255</v>
+        <v>1098677</v>
       </c>
       <c r="I58" s="2">
-        <f>8*G58/E58</f>
-        <v>1.9113220420829564</v>
+        <f t="shared" si="1"/>
+        <v>1.8948036031685636</v>
+      </c>
+      <c r="J58">
+        <v>2.27</v>
       </c>
       <c r="L58" t="s">
         <v>134</v>
       </c>
       <c r="M58" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.3">
@@ -3957,20 +3966,17 @@
         <v>4638695</v>
       </c>
       <c r="G59">
-        <v>1098677</v>
+        <v>1108255</v>
       </c>
       <c r="I59" s="2">
-        <f>8*G59/E59</f>
-        <v>1.8948036031685636</v>
-      </c>
-      <c r="J59">
-        <v>2.27</v>
+        <f t="shared" si="1"/>
+        <v>1.9113220420829564</v>
       </c>
       <c r="L59" t="s">
         <v>134</v>
       </c>
       <c r="M59" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.3">
@@ -3984,17 +3990,20 @@
         <v>4638695</v>
       </c>
       <c r="G60">
-        <v>1115894</v>
+        <v>1098677</v>
       </c>
       <c r="I60" s="2">
-        <f>8*G60/E60</f>
-        <v>1.9244964370367097</v>
+        <f t="shared" si="1"/>
+        <v>1.8948036031685636</v>
+      </c>
+      <c r="J60">
+        <v>2.27</v>
       </c>
       <c r="L60" t="s">
         <v>134</v>
       </c>
       <c r="M60" s="3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.3">
@@ -4008,29 +4017,23 @@
         <v>4638695</v>
       </c>
       <c r="G61">
-        <v>1109507</v>
+        <v>1115894</v>
       </c>
       <c r="I61" s="2">
-        <f>8*G61/E61</f>
-        <v>1.9134812700554789</v>
-      </c>
-      <c r="J61">
-        <v>3.27</v>
+        <f t="shared" si="1"/>
+        <v>1.9244964370367097</v>
       </c>
       <c r="L61" t="s">
         <v>134</v>
       </c>
       <c r="M61" s="3" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
         <v>62</v>
       </c>
-      <c r="C62" t="s">
-        <v>73</v>
-      </c>
       <c r="D62" t="s">
         <v>47</v>
       </c>
@@ -4038,25 +4041,28 @@
         <v>4638695</v>
       </c>
       <c r="G62">
-        <v>1129396</v>
+        <v>1109507</v>
       </c>
       <c r="I62" s="2">
-        <f>8*G62/E62</f>
-        <v>1.9477822965295195</v>
+        <f t="shared" si="1"/>
+        <v>1.9134812700554789</v>
       </c>
       <c r="J62">
-        <v>0.23</v>
+        <v>3.27</v>
       </c>
       <c r="L62" t="s">
         <v>134</v>
       </c>
       <c r="M62" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
-        <v>76</v>
+        <v>62</v>
+      </c>
+      <c r="C63" t="s">
+        <v>73</v>
       </c>
       <c r="D63" t="s">
         <v>47</v>
@@ -4065,25 +4071,25 @@
         <v>4638695</v>
       </c>
       <c r="G63">
-        <v>1109507</v>
+        <v>1129396</v>
       </c>
       <c r="I63" s="2">
-        <f>8*G63/E63</f>
-        <v>1.9134812700554789</v>
+        <f t="shared" si="1"/>
+        <v>1.9477822965295195</v>
+      </c>
+      <c r="J63">
+        <v>0.23</v>
       </c>
       <c r="L63" t="s">
         <v>134</v>
       </c>
+      <c r="M63" s="3" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
-        <v>79</v>
-      </c>
       <c r="B64" t="s">
-        <v>80</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D64" t="s">
         <v>47</v>
@@ -4092,22 +4098,25 @@
         <v>4638695</v>
       </c>
       <c r="G64">
-        <v>1115932</v>
+        <v>1109507</v>
       </c>
       <c r="I64" s="2">
-        <f>8*G64/E64</f>
-        <v>1.9245619727099972</v>
+        <f t="shared" si="1"/>
+        <v>1.9134812700554789</v>
       </c>
       <c r="L64" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>79</v>
+      </c>
       <c r="B65" t="s">
         <v>80</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D65" t="s">
         <v>47</v>
@@ -4116,11 +4125,11 @@
         <v>4638695</v>
       </c>
       <c r="G65">
-        <v>1117952</v>
+        <v>1115932</v>
       </c>
       <c r="I65" s="2">
-        <f>8*G65/E65</f>
-        <v>1.9280457111321179</v>
+        <f t="shared" si="1"/>
+        <v>1.9245619727099972</v>
       </c>
       <c r="L65" t="s">
         <v>135</v>
@@ -4131,7 +4140,7 @@
         <v>80</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D66" t="s">
         <v>47</v>
@@ -4140,11 +4149,11 @@
         <v>4638695</v>
       </c>
       <c r="G66">
-        <v>1112934</v>
+        <v>1117952</v>
       </c>
       <c r="I66" s="2">
-        <f>8*G66/E66</f>
-        <v>1.9193915530122156</v>
+        <f t="shared" si="1"/>
+        <v>1.9280457111321179</v>
       </c>
       <c r="L66" t="s">
         <v>135</v>
@@ -4155,7 +4164,7 @@
         <v>80</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D67" t="s">
         <v>47</v>
@@ -4164,38 +4173,32 @@
         <v>4638695</v>
       </c>
       <c r="G67">
-        <v>1097728</v>
+        <v>1112934</v>
       </c>
       <c r="I67" s="2">
-        <f>8*G67/E67</f>
-        <v>1.8931669359593593</v>
+        <f t="shared" si="1"/>
+        <v>1.9193915530122156</v>
       </c>
       <c r="L67" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
-        <v>85</v>
-      </c>
       <c r="B68" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D68" t="s">
-        <v>47</v>
+        <v>91</v>
       </c>
       <c r="E68">
         <v>4638695</v>
       </c>
       <c r="G68">
-        <v>1119377</v>
+        <v>1103429</v>
       </c>
       <c r="I68" s="2">
         <f>8*G68/E68</f>
-        <v>1.9305032988803963</v>
+        <v>1.9029990115754538</v>
       </c>
       <c r="L68" t="s">
         <v>135</v>
@@ -4203,10 +4206,10 @@
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D69" t="s">
         <v>47</v>
@@ -4215,22 +4218,25 @@
         <v>4638695</v>
       </c>
       <c r="G69">
-        <v>1118641</v>
+        <v>1097728</v>
       </c>
       <c r="I69" s="2">
-        <f>8*G69/E69</f>
-        <v>1.9292339763661979</v>
+        <f t="shared" si="1"/>
+        <v>1.8931669359593593</v>
       </c>
       <c r="L69" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>85</v>
+      </c>
       <c r="B70" t="s">
         <v>86</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D70" t="s">
         <v>47</v>
@@ -4239,11 +4245,11 @@
         <v>4638695</v>
       </c>
       <c r="G70">
-        <v>1119489</v>
+        <v>1119377</v>
       </c>
       <c r="I70" s="2">
-        <f>8*G70/E70</f>
-        <v>1.9306964566542961</v>
+        <f t="shared" si="1"/>
+        <v>1.9305032988803963</v>
       </c>
       <c r="L70" t="s">
         <v>135</v>
@@ -4254,7 +4260,7 @@
         <v>86</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D71" t="s">
         <v>47</v>
@@ -4263,11 +4269,11 @@
         <v>4638695</v>
       </c>
       <c r="G71">
-        <v>1113652</v>
+        <v>1118641</v>
       </c>
       <c r="I71" s="2">
-        <f>8*G71/E71</f>
-        <v>1.9206298323127518</v>
+        <f t="shared" si="1"/>
+        <v>1.9292339763661979</v>
       </c>
       <c r="L71" t="s">
         <v>135</v>
@@ -4278,7 +4284,7 @@
         <v>86</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D72" t="s">
         <v>47</v>
@@ -4287,11 +4293,11 @@
         <v>4638695</v>
       </c>
       <c r="G72">
-        <v>1116077</v>
+        <v>1119489</v>
       </c>
       <c r="I72" s="2">
-        <f>8*G72/E72</f>
-        <v>1.9248120430422782</v>
+        <f t="shared" ref="I72:I83" si="2">8*G72/E72</f>
+        <v>1.9306964566542961</v>
       </c>
       <c r="L72" t="s">
         <v>135</v>
@@ -4302,7 +4308,7 @@
         <v>86</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D73" t="s">
         <v>47</v>
@@ -4311,11 +4317,11 @@
         <v>4638695</v>
       </c>
       <c r="G73">
-        <v>1113065</v>
+        <v>1113652</v>
       </c>
       <c r="I73" s="2">
-        <f>8*G73/E73</f>
-        <v>1.9196174786227591</v>
+        <f t="shared" si="2"/>
+        <v>1.9206298323127518</v>
       </c>
       <c r="L73" t="s">
         <v>135</v>
@@ -4326,7 +4332,7 @@
         <v>86</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D74" t="s">
         <v>47</v>
@@ -4335,25 +4341,22 @@
         <v>4638695</v>
       </c>
       <c r="G74">
-        <v>1118316</v>
+        <v>1116077</v>
       </c>
       <c r="I74" s="2">
-        <f>8*G74/E74</f>
-        <v>1.9286734738972922</v>
+        <f t="shared" si="2"/>
+        <v>1.9248120430422782</v>
       </c>
       <c r="L74" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
-        <v>93</v>
-      </c>
       <c r="B75" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D75" t="s">
         <v>47</v>
@@ -4362,11 +4365,11 @@
         <v>4638695</v>
       </c>
       <c r="G75">
-        <v>1108978</v>
+        <v>1113065</v>
       </c>
       <c r="I75" s="2">
-        <f>8*G75/E75</f>
-        <v>1.9125689444983989</v>
+        <f t="shared" si="2"/>
+        <v>1.9196174786227591</v>
       </c>
       <c r="L75" t="s">
         <v>135</v>
@@ -4374,10 +4377,10 @@
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B76" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D76" t="s">
         <v>47</v>
@@ -4386,22 +4389,25 @@
         <v>4638695</v>
       </c>
       <c r="G76">
-        <v>1106151</v>
+        <v>1118316</v>
       </c>
       <c r="I76" s="2">
-        <f>8*G76/E76</f>
-        <v>1.9076934353304109</v>
+        <f t="shared" si="2"/>
+        <v>1.9286734738972922</v>
       </c>
       <c r="L76" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>93</v>
+      </c>
       <c r="B77" t="s">
         <v>94</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D77" t="s">
         <v>47</v>
@@ -4410,11 +4416,11 @@
         <v>4638695</v>
       </c>
       <c r="G77">
-        <v>1101875</v>
+        <v>1108978</v>
       </c>
       <c r="I77" s="2">
-        <f>8*G77/E77</f>
-        <v>1.9003189474625946</v>
+        <f t="shared" si="2"/>
+        <v>1.9125689444983989</v>
       </c>
       <c r="L77" t="s">
         <v>135</v>
@@ -4425,7 +4431,7 @@
         <v>94</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D78" t="s">
         <v>47</v>
@@ -4434,11 +4440,11 @@
         <v>4638695</v>
       </c>
       <c r="G78">
-        <v>1112676</v>
+        <v>1106151</v>
       </c>
       <c r="I78" s="2">
-        <f>8*G78/E78</f>
-        <v>1.9189466002830537</v>
+        <f t="shared" si="2"/>
+        <v>1.9076934353304109</v>
       </c>
       <c r="L78" t="s">
         <v>135</v>
@@ -4449,7 +4455,7 @@
         <v>94</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D79" t="s">
         <v>47</v>
@@ -4458,11 +4464,11 @@
         <v>4638695</v>
       </c>
       <c r="G79">
-        <v>1109196</v>
+        <v>1101875</v>
       </c>
       <c r="I79" s="2">
         <f>8*G79/E79</f>
-        <v>1.9129449123083109</v>
+        <v>1.9003189474625946</v>
       </c>
       <c r="L79" t="s">
         <v>135</v>
@@ -4473,7 +4479,7 @@
         <v>94</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D80" t="s">
         <v>47</v>
@@ -4482,22 +4488,22 @@
         <v>4638695</v>
       </c>
       <c r="G80">
-        <v>1114590</v>
+        <v>1112676</v>
       </c>
       <c r="I80" s="2">
-        <f>8*G80/E80</f>
-        <v>1.9222475286691623</v>
+        <f t="shared" si="2"/>
+        <v>1.9189466002830537</v>
       </c>
       <c r="L80" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
-        <v>77</v>
-      </c>
       <c r="B81" t="s">
-        <v>78</v>
+        <v>94</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>97</v>
       </c>
       <c r="D81" t="s">
         <v>47</v>
@@ -4506,13 +4512,61 @@
         <v>4638695</v>
       </c>
       <c r="G81">
+        <v>1109196</v>
+      </c>
+      <c r="I81" s="2">
+        <f t="shared" si="2"/>
+        <v>1.9129449123083109</v>
+      </c>
+      <c r="L81" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B82" t="s">
+        <v>94</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D82" t="s">
+        <v>47</v>
+      </c>
+      <c r="E82">
+        <v>4638695</v>
+      </c>
+      <c r="G82">
+        <v>1114590</v>
+      </c>
+      <c r="I82" s="2">
+        <f t="shared" si="2"/>
+        <v>1.9222475286691623</v>
+      </c>
+      <c r="L82" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>77</v>
+      </c>
+      <c r="B83" t="s">
+        <v>78</v>
+      </c>
+      <c r="D83" t="s">
+        <v>47</v>
+      </c>
+      <c r="E83">
+        <v>4638695</v>
+      </c>
+      <c r="G83">
         <v>1123789</v>
       </c>
-      <c r="I81" s="2">
-        <f>8*G81/E81</f>
+      <c r="I83" s="2">
+        <f t="shared" si="2"/>
         <v>1.9381123354736622</v>
       </c>
-      <c r="L81" t="s">
+      <c r="L83" t="s">
         <v>135</v>
       </c>
     </row>
@@ -4529,8 +4583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9596547-0124-4F45-A588-1674B314477A}">
   <dimension ref="A2:I33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView topLeftCell="B16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="U33" sqref="U33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>